<commit_message>
excel html works with check availability
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/command_results.xlsx
+++ b/ExportedFiles/excelFiles/command_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,16 +464,6 @@
           <t>Entered Time</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Date Entered?</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Time Entered?</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -498,8 +488,6 @@
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -532,14 +520,228 @@
           <t>15:22:00</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Yes</t>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-09-09 15:28:31</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>15:28:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-09-09 15:34:29</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>15:34:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-09-09 15:38:11</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>15:38:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-09-09 15:40:38</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>15:40:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-09-09 15:43:17</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>15:43:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-09-09 15:44:02</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>15:44:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-09-09 15:45:01</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>check_availability</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>No availability for the selected date.</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>15:45:01</t>
         </is>
       </c>
     </row>

</xml_diff>